<commit_message>
remember when i said no more code? I LIED
</commit_message>
<xml_diff>
--- a/code/matlab_testerino/stored probability.xlsx
+++ b/code/matlab_testerino/stored probability.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17127"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carpanta\Documents\GitHub\tiic-2015\code\matlab_testerino\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\GitHub\tiic-2015\code\matlab_testerino\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>P(x4)</t>
   </si>
@@ -63,21 +63,6 @@
   </si>
   <si>
     <t>P(x1)</t>
-  </si>
-  <si>
-    <t>-0,0628215282355947, -0,900532690625621, -2,06730257227987, -3,44012693636725, -4,97007472043432, -6,63169462376867, -8,41028433404004, -10,2972135191002, -12,2878921416988, -14,3808758091921, -16,5776089142238, -18,8826814940444, -21,3047238808019, -23,8584383868268, -26,5692763128313, -29,4861687212689, -32,7321198489708</t>
-  </si>
-  <si>
-    <t>-0,126216195408805, -0,658935195436524, -1,52071291472847, -2,58854511645354, -3,81350073815831, -5,17012847913034, -6,64372602703941, -8,2256630497373, -9,91134950997357, -11,6993410151046, -13,591081957774, -15,5911623752322, -17,7082125996275, -19,95693494329, -22,3627807069322, -24,9746809530075, -27,9156399183471</t>
-  </si>
-  <si>
-    <t>-0,276425797303274, -0,463964595289396, -0,980562112539742, -1,70321411222321, -2,58298953188638, -3,59443707081682, -4,72285441668429, -5,95961123734059, -7,30011749553526, -8,74292879862468, -10,2894895392525, -11,9443897546691, -13,7162597770228, -15,6198019186437, -17,6804674802443, -19,947187524278, -22,542966287576</t>
-  </si>
-  <si>
-    <t>-0,579394762471116, -0,435972620168803, -0,621609197130714, -1,01330025652575, -1,56211473590049, -2,24260133454249, -3,04005774012152, -3,94585362048939, -4,95539893839562, -6,06724930119662, -7,28284910153597, -8,60678837666416, -10,0476974587294, -11,6202786600619, -13,3499832813741, -15,2857423851194, -17,5505602081289</t>
-  </si>
-  <si>
-    <t>-4,8164799306237, -3,61235994796777, -2,73729868457607, -2,0682919036175, -1,55640854263862, -1,17619730092702, -0,912955866152437, -0,758053906166694, -0,706901383719312, -0,758053906166694, -0,912955866152437, -1,17619730092702, -1,55640854263862, -2,0682919036175, -2,73729868457607, -3,61235994796777, -4,8164799306237</t>
   </si>
 </sst>
 </file>
@@ -147,7 +132,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -736,7 +720,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1371,7 +1354,7 @@
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>100012</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1470,6 +1453,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1505,6 +1505,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1657,10 +1674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R35"/>
+  <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2126,818 +2143,1144 @@
         <v>1.5258789062500007E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15">
-        <f>LOG(B8)</f>
-        <v>-6.282152823559474E-2</v>
-      </c>
-      <c r="C15">
-        <f t="shared" ref="C15:Q15" si="5">LOG(C8)</f>
-        <v>-0.90053269062562058</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="5"/>
-        <v>-2.0673025722798708</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="5"/>
-        <v>-3.4401269363672458</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="5"/>
-        <v>-4.9700747204343214</v>
-      </c>
-      <c r="G15">
-        <f t="shared" si="5"/>
-        <v>-6.6316946237686665</v>
-      </c>
-      <c r="H15">
-        <f t="shared" si="5"/>
-        <v>-8.4102843340400355</v>
-      </c>
-      <c r="I15">
-        <f t="shared" si="5"/>
-        <v>-10.297213519100243</v>
-      </c>
-      <c r="J15">
-        <f t="shared" si="5"/>
-        <v>-12.28789214169881</v>
-      </c>
-      <c r="K15">
-        <f t="shared" si="5"/>
-        <v>-14.380875809192142</v>
-      </c>
-      <c r="L15">
-        <f t="shared" si="5"/>
-        <v>-16.577608914223838</v>
-      </c>
-      <c r="M15">
-        <f t="shared" si="5"/>
-        <v>-18.882681494044366</v>
-      </c>
-      <c r="N15">
-        <f t="shared" si="5"/>
-        <v>-21.304723880801927</v>
-      </c>
-      <c r="O15">
-        <f t="shared" si="5"/>
-        <v>-23.858438386826752</v>
-      </c>
-      <c r="P15">
-        <f t="shared" si="5"/>
-        <v>-26.569276312831274</v>
-      </c>
-      <c r="Q15">
-        <f t="shared" si="5"/>
-        <v>-29.486168721268925</v>
-      </c>
-      <c r="R15">
-        <f t="shared" ref="R15" si="6">LOG(R8)</f>
-        <v>-32.732119848970804</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16">
-        <f t="shared" ref="B16:Q16" si="7">LOG(B9)</f>
-        <v>-0.1262161954088053</v>
-      </c>
-      <c r="C16">
-        <f t="shared" si="7"/>
-        <v>-0.65893519543652423</v>
-      </c>
-      <c r="D16">
-        <f t="shared" si="7"/>
-        <v>-1.5207129147284679</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="7"/>
-        <v>-2.5885451164535356</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="7"/>
-        <v>-3.8135007381583055</v>
-      </c>
-      <c r="G16">
-        <f t="shared" si="7"/>
-        <v>-5.1701284791303426</v>
-      </c>
-      <c r="H16">
-        <f t="shared" si="7"/>
-        <v>-6.6437260270394054</v>
-      </c>
-      <c r="I16">
-        <f t="shared" si="7"/>
-        <v>-8.2256630497373049</v>
-      </c>
-      <c r="J16">
-        <f t="shared" si="7"/>
-        <v>-9.9113495099735669</v>
-      </c>
-      <c r="K16">
-        <f t="shared" si="7"/>
-        <v>-11.699341015104592</v>
-      </c>
-      <c r="L16">
-        <f t="shared" si="7"/>
-        <v>-13.591081957773978</v>
-      </c>
-      <c r="M16">
-        <f t="shared" si="7"/>
-        <v>-15.591162375232207</v>
-      </c>
-      <c r="N16">
-        <f t="shared" si="7"/>
-        <v>-17.708212599627451</v>
-      </c>
-      <c r="O16">
-        <f t="shared" si="7"/>
-        <v>-19.956934943289976</v>
-      </c>
-      <c r="P16">
-        <f t="shared" si="7"/>
-        <v>-22.362780706932195</v>
-      </c>
-      <c r="Q16">
-        <f t="shared" si="7"/>
-        <v>-24.974680953007535</v>
-      </c>
-      <c r="R16">
-        <f t="shared" ref="R16" si="8">LOG(R9)</f>
-        <v>-27.915639918347104</v>
-      </c>
-    </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>8</v>
-      </c>
       <c r="B17">
-        <f t="shared" ref="B17:Q17" si="9">LOG(B10)</f>
-        <v>-0.27642579730327427</v>
-      </c>
-      <c r="C17">
-        <f t="shared" si="9"/>
-        <v>-0.46396459528939565</v>
-      </c>
-      <c r="D17">
-        <f t="shared" si="9"/>
-        <v>-0.98056211253974168</v>
-      </c>
-      <c r="E17">
-        <f t="shared" si="9"/>
-        <v>-1.7032141122232123</v>
-      </c>
-      <c r="F17">
-        <f t="shared" si="9"/>
-        <v>-2.5829895318863842</v>
-      </c>
-      <c r="G17">
-        <f t="shared" si="9"/>
-        <v>-3.5944370708168241</v>
-      </c>
-      <c r="H17">
-        <f t="shared" si="9"/>
-        <v>-4.7228544166842878</v>
-      </c>
-      <c r="I17">
-        <f t="shared" si="9"/>
-        <v>-5.9596112373405914</v>
-      </c>
-      <c r="J17">
-        <f t="shared" si="9"/>
-        <v>-7.3001174955352575</v>
-      </c>
-      <c r="K17">
-        <f t="shared" si="9"/>
-        <v>-8.7429287986246838</v>
-      </c>
-      <c r="L17">
-        <f t="shared" si="9"/>
-        <v>-10.289489539252472</v>
-      </c>
-      <c r="M17">
-        <f t="shared" si="9"/>
-        <v>-11.944389754669103</v>
-      </c>
-      <c r="N17">
-        <f t="shared" si="9"/>
-        <v>-13.716259777022753</v>
-      </c>
-      <c r="O17">
-        <f t="shared" si="9"/>
-        <v>-15.619801918643676</v>
-      </c>
-      <c r="P17">
-        <f t="shared" si="9"/>
-        <v>-17.680467480244296</v>
-      </c>
-      <c r="Q17">
-        <f t="shared" si="9"/>
-        <v>-19.947187524278043</v>
-      </c>
-      <c r="R17">
-        <f t="shared" ref="R17" si="10">LOG(R10)</f>
-        <v>-22.542966287576011</v>
+        <f>B8</f>
+        <v>0.86532344729557997</v>
+      </c>
+      <c r="C17" t="str">
+        <f>CONCATENATE(B17,", ",C8)</f>
+        <v>0,86532344729558, 0,12573822039411</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" ref="D17:D21" si="5">CONCATENATE(C17,", ",D8)</f>
+        <v>0,86532344729558, 0,12573822039411, 0,00856440956266646</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" ref="E17:E21" si="6">CONCATENATE(D17,", ",E8)</f>
+        <v>0,86532344729558, 0,12573822039411, 0,00856440956266646, 0,000362971949174562</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" ref="F17:F21" si="7">CONCATENATE(E17,", ",F8)</f>
+        <v>0,86532344729558, 0,12573822039411, 0,00856440956266646, 0,000362971949174562, 1,07133496602986E-05</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" ref="G17:G21" si="8">CONCATENATE(F17,", ",G8)</f>
+        <v>0,86532344729558, 0,12573822039411, 0,00856440956266646, 0,000362971949174562, 1,07133496602986E-05, 2,33509942141726E-07</v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" ref="H17:H21" si="9">CONCATENATE(G17,", ",H8)</f>
+        <v>0,86532344729558, 0,12573822039411, 0,00856440956266646, 0,000362971949174562, 1,07133496602986E-05, 2,33509942141726E-07, 3,88790519206709E-09</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" ref="I17:I21" si="10">CONCATENATE(H17,", ",I8)</f>
+        <v>0,86532344729558, 0,12573822039411, 0,00856440956266646, 0,000362971949174562, 1,07133496602986E-05, 2,33509942141726E-07, 3,88790519206709E-09, 5,04413243889342E-11</v>
+      </c>
+      <c r="J17" t="str">
+        <f t="shared" ref="J17:J21" si="11">CONCATENATE(I17,", ",J8)</f>
+        <v>0,86532344729558, 0,12573822039411, 0,00856440956266646, 0,000362971949174562, 1,07133496602986E-05, 2,33509942141726E-07, 3,88790519206709E-09, 5,04413243889342E-11, 5,15356619009042E-13</v>
+      </c>
+      <c r="K17" t="str">
+        <f t="shared" ref="K17:K21" si="12">CONCATENATE(J17,", ",K8)</f>
+        <v>0,86532344729558, 0,12573822039411, 0,00856440956266646, 0,000362971949174562, 1,07133496602986E-05, 2,33509942141726E-07, 3,88790519206709E-09, 5,04413243889342E-11, 5,15356619009042E-13, 4,16029561258561E-15</v>
+      </c>
+      <c r="L17" t="str">
+        <f t="shared" ref="L17:L21" si="13">CONCATENATE(K17,", ",L8)</f>
+        <v>0,86532344729558, 0,12573822039411, 0,00856440956266646, 0,000362971949174562, 1,07133496602986E-05, 2,33509942141726E-07, 3,88790519206709E-09, 5,04413243889342E-11, 5,15356619009042E-13, 4,16029561258561E-15, 2,64478933998883E-17</v>
+      </c>
+      <c r="M17" t="str">
+        <f t="shared" ref="M17:M21" si="14">CONCATENATE(L17,", ",M8)</f>
+        <v>0,86532344729558, 0,12573822039411, 0,00856440956266646, 0,000362971949174562, 1,07133496602986E-05, 2,33509942141726E-07, 3,88790519206709E-09, 5,04413243889342E-11, 5,15356619009042E-13, 4,16029561258561E-15, 2,64478933998883E-17, 1,31014241225023E-19</v>
+      </c>
+      <c r="N17" t="str">
+        <f t="shared" ref="N17:N21" si="15">CONCATENATE(M17,", ",N8)</f>
+        <v>0,86532344729558, 0,12573822039411, 0,00856440956266646, 0,000362971949174562, 1,07133496602986E-05, 2,33509942141726E-07, 3,88790519206709E-09, 5,04413243889342E-11, 5,15356619009042E-13, 4,16029561258561E-15, 2,64478933998883E-17, 1,31014241225023E-19, 4,95765292223848E-22</v>
+      </c>
+      <c r="O17" t="str">
+        <f t="shared" ref="O17:O21" si="16">CONCATENATE(N17,", ",O8)</f>
+        <v>0,86532344729558, 0,12573822039411, 0,00856440956266646, 0,000362971949174562, 1,07133496602986E-05, 2,33509942141726E-07, 3,88790519206709E-09, 5,04413243889342E-11, 5,15356619009042E-13, 4,16029561258561E-15, 2,64478933998883E-17, 1,31014241225023E-19, 4,95765292223848E-22, 1,38535671195051E-24</v>
+      </c>
+      <c r="P17" t="str">
+        <f t="shared" ref="P17:P21" si="17">CONCATENATE(O17,", ",P8)</f>
+        <v>0,86532344729558, 0,12573822039411, 0,00856440956266646, 0,000362971949174562, 1,07133496602986E-05, 2,33509942141726E-07, 3,88790519206709E-09, 5,04413243889342E-11, 5,15356619009042E-13, 4,16029561258561E-15, 2,64478933998883E-17, 1,31014241225023E-19, 4,95765292223848E-22, 1,38535671195051E-24, 2,69602358531527E-27</v>
+      </c>
+      <c r="Q17" t="str">
+        <f t="shared" ref="Q17:Q21" si="18">CONCATENATE(P17,", ",Q8)</f>
+        <v>0,86532344729558, 0,12573822039411, 0,00856440956266646, 0,000362971949174562, 1,07133496602986E-05, 2,33509942141726E-07, 3,88790519206709E-09, 5,04413243889342E-11, 5,15356619009042E-13, 4,16029561258561E-15, 2,64478933998883E-17, 1,31014241225023E-19, 4,95765292223848E-22, 1,38535671195051E-24, 2,69602358531527E-27, 3,26460979049277E-30</v>
+      </c>
+      <c r="R17" t="str">
+        <f t="shared" ref="R17:R21" si="19">CONCATENATE(Q17,", ",R8)</f>
+        <v>0,86532344729558, 0,12573822039411, 0,00856440956266646, 0,000362971949174562, 1,07133496602986E-05, 2,33509942141726E-07, 3,88790519206709E-09, 5,04413243889342E-11, 5,15356619009042E-13, 4,16029561258561E-15, 2,64478933998883E-17, 1,31014241225023E-19, 4,95765292223848E-22, 1,38535671195051E-24, 2,69602358531527E-27, 3,26460979049277E-30, 1,85302018885184E-33</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>8</v>
-      </c>
       <c r="B18">
-        <f t="shared" ref="B18:Q18" si="11">LOG(B11)</f>
-        <v>-0.57939476247111577</v>
-      </c>
-      <c r="C18">
+        <f t="shared" ref="B18:B21" si="20">B9</f>
+        <v>0.74779714819265464</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" ref="C18:C21" si="21">CONCATENATE(B18,", ",C9)</f>
+        <v>0,747797148192655, 0,219313216577886</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="5"/>
+        <v>0,747797148192655, 0,219313216577886, 0,0301499839490984</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="6"/>
+        <v>0,747797148192655, 0,219313216577886, 0,0301499839490984, 0,00257902103026911</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="7"/>
+        <v>0,747797148192655, 0,219313216577886, 0,0301499839490984, 0,00257902103026911, 0,000153638218198313</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="8"/>
+        <v>0,747797148192655, 0,219313216577886, 0,0301499839490984, 0,00257902103026911, 0,000153638218198313, 6,75882996554695E-06</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="9"/>
+        <v>0,747797148192655, 0,219313216577886, 0,0301499839490984, 0,00257902103026911, 0,000153638218198313, 6,75882996554695E-06, 2,27129723893126E-07</v>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" si="10"/>
+        <v>0,747797148192655, 0,219313216577886, 0,0301499839490984, 0,00257902103026911, 0,000153638218198313, 6,75882996554695E-06, 2,27129723893126E-07, 5,94753423054447E-09</v>
+      </c>
+      <c r="J18" t="str">
         <f t="shared" si="11"/>
-        <v>-0.43597262016880262</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="11"/>
-        <v>-0.62160919713071427</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="11"/>
-        <v>-1.0133002565257505</v>
-      </c>
-      <c r="F18">
-        <f t="shared" si="11"/>
-        <v>-1.5621147359004877</v>
-      </c>
-      <c r="G18">
-        <f t="shared" si="11"/>
-        <v>-2.2426013345424933</v>
-      </c>
-      <c r="H18">
-        <f t="shared" si="11"/>
-        <v>-3.0400577401215236</v>
-      </c>
-      <c r="I18">
-        <f t="shared" si="11"/>
-        <v>-3.9458536204893924</v>
-      </c>
-      <c r="J18">
-        <f t="shared" si="11"/>
-        <v>-4.9553989383956232</v>
-      </c>
-      <c r="K18">
-        <f t="shared" si="11"/>
-        <v>-6.0672493011966155</v>
-      </c>
-      <c r="L18">
-        <f t="shared" si="11"/>
-        <v>-7.2828491015359713</v>
-      </c>
-      <c r="M18">
-        <f t="shared" si="11"/>
-        <v>-8.6067883766641646</v>
-      </c>
-      <c r="N18">
-        <f t="shared" si="11"/>
-        <v>-10.047697458729381</v>
-      </c>
-      <c r="O18">
-        <f t="shared" si="11"/>
-        <v>-11.620278660061865</v>
-      </c>
-      <c r="P18">
-        <f t="shared" si="11"/>
-        <v>-13.349983281374056</v>
-      </c>
-      <c r="Q18">
-        <f t="shared" si="11"/>
-        <v>-15.285742385119367</v>
-      </c>
-      <c r="R18">
-        <f t="shared" ref="R18" si="12">LOG(R11)</f>
-        <v>-17.550560208128903</v>
+        <v>0,747797148192655, 0,219313216577886, 0,0301499839490984, 0,00257902103026911, 0,000153638218198313, 6,75882996554695E-06, 2,27129723893126E-07, 5,94753423054447E-09, 1,22645181434344E-10</v>
+      </c>
+      <c r="K18" t="str">
+        <f t="shared" si="12"/>
+        <v>0,747797148192655, 0,219313216577886, 0,0301499839490984, 0,00257902103026911, 0,000153638218198313, 6,75882996554695E-06, 2,27129723893126E-07, 5,94753423054447E-09, 1,22645181434344E-10, 1,99829216186303E-12</v>
+      </c>
+      <c r="L18" t="str">
+        <f t="shared" si="13"/>
+        <v>0,747797148192655, 0,219313216577886, 0,0301499839490984, 0,00257902103026911, 0,000153638218198313, 6,75882996554695E-06, 2,27129723893126E-07, 5,94753423054447E-09, 1,22645181434344E-10, 1,99829216186303E-12, 2,56400012621938E-14</v>
+      </c>
+      <c r="M18" t="str">
+        <f t="shared" si="14"/>
+        <v>0,747797148192655, 0,219313216577886, 0,0301499839490984, 0,00257902103026911, 0,000153638218198313, 6,75882996554695E-06, 2,27129723893126E-07, 5,94753423054447E-09, 1,22645181434344E-10, 1,99829216186303E-12, 2,56400012621938E-14, 2,56352539929356E-16</v>
+      </c>
+      <c r="N18" t="str">
+        <f t="shared" si="15"/>
+        <v>0,747797148192655, 0,219313216577886, 0,0301499839490984, 0,00257902103026911, 0,000153638218198313, 6,75882996554695E-06, 2,27129723893126E-07, 5,94753423054447E-09, 1,22645181434344E-10, 1,99829216186303E-12, 2,56400012621938E-14, 2,56352539929356E-16, 1,95788599742381E-18</v>
+      </c>
+      <c r="O18" t="str">
+        <f t="shared" si="16"/>
+        <v>0,747797148192655, 0,219313216577886, 0,0301499839490984, 0,00257902103026911, 0,000153638218198313, 6,75882996554695E-06, 2,27129723893126E-07, 5,94753423054447E-09, 1,22645181434344E-10, 1,99829216186303E-12, 2,56400012621938E-14, 2,56352539929356E-16, 1,95788599742381E-18, 1,10424402173362E-20</v>
+      </c>
+      <c r="P18" t="str">
+        <f t="shared" si="17"/>
+        <v>0,747797148192655, 0,219313216577886, 0,0301499839490984, 0,00257902103026911, 0,000153638218198313, 6,75882996554695E-06, 2,27129723893126E-07, 5,94753423054447E-09, 1,22645181434344E-10, 1,99829216186303E-12, 2,56400012621938E-14, 2,56352539929356E-16, 1,95788599742381E-18, 1,10424402173362E-20, 4,33729831056261E-23</v>
+      </c>
+      <c r="Q18" t="str">
+        <f t="shared" si="18"/>
+        <v>0,747797148192655, 0,219313216577886, 0,0301499839490984, 0,00257902103026911, 0,000153638218198313, 6,75882996554695E-06, 2,27129723893126E-07, 5,94753423054447E-09, 1,22645181434344E-10, 1,99829216186303E-12, 2,56400012621938E-14, 2,56352539929356E-16, 1,95788599742381E-18, 1,10424402173362E-20, 4,33729831056261E-23, 1,06003217366094E-25</v>
+      </c>
+      <c r="R18" t="str">
+        <f t="shared" si="19"/>
+        <v>0,747797148192655, 0,219313216577886, 0,0301499839490984, 0,00257902103026911, 0,000153638218198313, 6,75882996554695E-06, 2,27129723893126E-07, 5,94753423054447E-09, 1,22645181434344E-10, 1,99829216186303E-12, 2,56400012621938E-14, 2,56352539929356E-16, 1,95788599742381E-18, 1,10424402173362E-20, 4,33729831056261E-23, 1,06003217366094E-25, 1,21439531096594E-28</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>10</v>
-      </c>
       <c r="B19">
-        <f t="shared" ref="B19:Q19" si="13">LOG(B12)</f>
-        <v>-4.8164799306236992</v>
-      </c>
-      <c r="C19">
+        <f t="shared" si="20"/>
+        <v>0.52914439805242031</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="21"/>
+        <v>0,52914439805242, 0,343585956695848</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="5"/>
+        <v>0,52914439805242, 0,343585956695848, 0,104577411377248</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="6"/>
+        <v>0,52914439805242, 0,343585956695848, 0,104577411377248, 0,0198055035074497</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="7"/>
+        <v>0,52914439805242, 0,343585956695848, 0,104577411377248, 0,0198055035074497, 0,00261222431797009</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="8"/>
+        <v>0,52914439805242, 0,343585956695848, 0,104577411377248, 0,0198055035074497, 0,00261222431797009, 0,000254426843040583</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="9"/>
+        <v>0,52914439805242, 0,343585956695848, 0,104577411377248, 0,0198055035074497, 0,00261222431797009, 0,000254426843040583, 1,89297807257042E-05</v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" si="10"/>
+        <v>0,52914439805242, 0,343585956695848, 0,104577411377248, 0,0198055035074497, 0,00261222431797009, 0,000254426843040583, 1,89297807257042E-05, 1,09746015802358E-06</v>
+      </c>
+      <c r="J19" t="str">
+        <f t="shared" si="11"/>
+        <v>0,52914439805242, 0,343585956695848, 0,104577411377248, 0,0198055035074497, 0,00261222431797009, 0,000254426843040583, 1,89297807257042E-05, 1,09746015802358E-06, 5,01051659035218E-08</v>
+      </c>
+      <c r="K19" t="str">
+        <f t="shared" si="12"/>
+        <v>0,52914439805242, 0,343585956695848, 0,104577411377248, 0,0198055035074497, 0,00261222431797009, 0,000254426843040583, 1,89297807257042E-05, 1,09746015802358E-06, 5,01051659035218E-08, 1,80747043148327E-09</v>
+      </c>
+      <c r="L19" t="str">
         <f t="shared" si="13"/>
-        <v>-3.6123599479677737</v>
-      </c>
-      <c r="D19">
+        <v>0,52914439805242, 0,343585956695848, 0,104577411377248, 0,0198055035074497, 0,00261222431797009, 0,000254426843040583, 1,89297807257042E-05, 1,09746015802358E-06, 5,01051659035218E-08, 1,80747043148327E-09, 5,13464545051961E-11</v>
+      </c>
+      <c r="M19" t="str">
+        <f t="shared" si="14"/>
+        <v>0,52914439805242, 0,343585956695848, 0,104577411377248, 0,0198055035074497, 0,00261222431797009, 0,000254426843040583, 1,89297807257042E-05, 1,09746015802358E-06, 5,01051659035218E-08, 1,80747043148327E-09, 5,13464545051961E-11, 1,13660678783614E-12</v>
+      </c>
+      <c r="N19" t="str">
+        <f t="shared" si="15"/>
+        <v>0,52914439805242, 0,343585956695848, 0,104577411377248, 0,0198055035074497, 0,00261222431797009, 0,000254426843040583, 1,89297807257042E-05, 1,09746015802358E-06, 5,01051659035218E-08, 1,80747043148327E-09, 5,13464545051961E-11, 1,13660678783614E-12, 1,92194175882802E-14</v>
+      </c>
+      <c r="O19" t="str">
+        <f t="shared" si="16"/>
+        <v>0,52914439805242, 0,343585956695848, 0,104577411377248, 0,0198055035074497, 0,00261222431797009, 0,000254426843040583, 1,89297807257042E-05, 1,09746015802358E-06, 5,01051659035218E-08, 1,80747043148327E-09, 5,13464545051961E-11, 1,13660678783614E-12, 1,92194175882802E-14, 2,39992727429097E-16</v>
+      </c>
+      <c r="P19" t="str">
+        <f t="shared" si="17"/>
+        <v>0,52914439805242, 0,343585956695848, 0,104577411377248, 0,0198055035074497, 0,00261222431797009, 0,000254426843040583, 1,89297807257042E-05, 1,09746015802358E-06, 5,01051659035218E-08, 1,80747043148327E-09, 5,13464545051961E-11, 1,13660678783614E-12, 1,92194175882802E-14, 2,39992727429097E-16, 2,08704839521365E-18</v>
+      </c>
+      <c r="Q19" t="str">
+        <f t="shared" si="18"/>
+        <v>0,52914439805242, 0,343585956695848, 0,104577411377248, 0,0198055035074497, 0,00261222431797009, 0,000254426843040583, 1,89297807257042E-05, 1,09746015802358E-06, 5,01051659035218E-08, 1,80747043148327E-09, 5,13464545051961E-11, 1,13660678783614E-12, 1,92194175882802E-14, 2,39992727429097E-16, 2,08704839521365E-18, 1,12930818471498E-20</v>
+      </c>
+      <c r="R19" t="str">
+        <f t="shared" si="19"/>
+        <v>0,52914439805242, 0,343585956695848, 0,104577411377248, 0,0198055035074497, 0,00261222431797009, 0,000254426843040583, 1,89297807257042E-05, 1,09746015802358E-06, 5,01051659035218E-08, 1,80747043148327E-09, 5,13464545051961E-11, 1,13660678783614E-12, 1,92194175882802E-14, 2,39992727429097E-16, 2,08704839521365E-18, 1,12930818471498E-20, 2,86440031242744E-23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <f t="shared" si="20"/>
+        <v>0.26339361174458853</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="21"/>
+        <v>0,263393611744589, 0,366460677209862</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="5"/>
+        <v>0,263393611744589, 0,366460677209862, 0,238996093832519</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="6"/>
+        <v>0,263393611744589, 0,366460677209862, 0,238996093832519, 0,0969839221349352</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="7"/>
+        <v>0,263393611744589, 0,366460677209862, 0,238996093832519, 0,0969839221349352, 0,027408499733786</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="8"/>
+        <v>0,263393611744589, 0,366460677209862, 0,238996093832519, 0,0969839221349352, 0,027408499733786, 0,005720034727051</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="9"/>
+        <v>0,263393611744589, 0,366460677209862, 0,238996093832519, 0,0969839221349352, 0,027408499733786, 0,005720034727051, 0,00091188959416755</v>
+      </c>
+      <c r="I20" t="str">
+        <f t="shared" si="10"/>
+        <v>0,263393611744589, 0,366460677209862, 0,238996093832519, 0,0969839221349352, 0,027408499733786, 0,005720034727051, 0,00091188959416755, 0,000113278210455596</v>
+      </c>
+      <c r="J20" t="str">
+        <f t="shared" si="11"/>
+        <v>0,263393611744589, 0,366460677209862, 0,238996093832519, 0,0969839221349352, 0,027408499733786, 0,005720034727051, 0,00091188959416755, 0,000113278210455596, 1,10815640663083E-05</v>
+      </c>
+      <c r="K20" t="str">
+        <f t="shared" si="12"/>
+        <v>0,263393611744589, 0,366460677209862, 0,238996093832519, 0,0969839221349352, 0,027408499733786, 0,005720034727051, 0,00091188959416755, 0,000113278210455596, 1,10815640663083E-05, 8,56546014787117E-07</v>
+      </c>
+      <c r="L20" t="str">
         <f t="shared" si="13"/>
-        <v>-2.7372986845760741</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="13"/>
-        <v>-2.0682919036174989</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="13"/>
-        <v>-1.5564085426386243</v>
-      </c>
-      <c r="G19">
-        <f t="shared" si="13"/>
-        <v>-1.1761973009270184</v>
-      </c>
-      <c r="H19">
-        <f t="shared" si="13"/>
-        <v>-0.91295586615243696</v>
-      </c>
-      <c r="I19">
-        <f t="shared" si="13"/>
-        <v>-0.75805390616669377</v>
-      </c>
-      <c r="J19">
-        <f t="shared" si="13"/>
-        <v>-0.70690138371931244</v>
-      </c>
-      <c r="K19">
-        <f t="shared" si="13"/>
-        <v>-0.75805390616669377</v>
-      </c>
-      <c r="L19">
-        <f t="shared" si="13"/>
-        <v>-0.91295586615243696</v>
-      </c>
-      <c r="M19">
-        <f t="shared" si="13"/>
-        <v>-1.1761973009270184</v>
-      </c>
-      <c r="N19">
-        <f t="shared" si="13"/>
-        <v>-1.5564085426386243</v>
-      </c>
-      <c r="O19">
-        <f t="shared" si="13"/>
-        <v>-2.0682919036174994</v>
-      </c>
-      <c r="P19">
-        <f t="shared" si="13"/>
-        <v>-2.7372986845760741</v>
-      </c>
-      <c r="Q19">
-        <f t="shared" si="13"/>
-        <v>-3.6123599479677737</v>
-      </c>
-      <c r="R19">
-        <f t="shared" ref="R19" si="14">LOG(R12)</f>
-        <v>-4.8164799306236992</v>
+        <v>0,263393611744589, 0,366460677209862, 0,238996093832519, 0,0969839221349352, 0,027408499733786, 0,005720034727051, 0,00091188959416755, 0,000113278210455596, 1,10815640663083E-05, 8,56546014787117E-07, 5,2137583508781E-08</v>
+      </c>
+      <c r="M20" t="str">
+        <f t="shared" si="14"/>
+        <v>0,263393611744589, 0,366460677209862, 0,238996093832519, 0,0969839221349352, 0,027408499733786, 0,005720034727051, 0,00091188959416755, 0,000113278210455596, 1,10815640663083E-05, 8,56546014787117E-07, 5,2137583508781E-08, 2,47292886207657E-09</v>
+      </c>
+      <c r="N20" t="str">
+        <f t="shared" si="15"/>
+        <v>0,263393611744589, 0,366460677209862, 0,238996093832519, 0,0969839221349352, 0,027408499733786, 0,005720034727051, 0,00091188959416755, 0,000113278210455596, 1,10815640663083E-05, 8,56546014787117E-07, 5,2137583508781E-08, 2,47292886207657E-09, 8,95988718143687E-11</v>
+      </c>
+      <c r="O20" t="str">
+        <f t="shared" si="16"/>
+        <v>0,263393611744589, 0,366460677209862, 0,238996093832519, 0,0969839221349352, 0,027408499733786, 0,005720034727051, 0,00091188959416755, 0,000113278210455596, 1,10815640663083E-05, 8,56546014787117E-07, 5,2137583508781E-08, 2,47292886207657E-09, 8,95988718143687E-11, 2,39729422914699E-12</v>
+      </c>
+      <c r="P20" t="str">
+        <f t="shared" si="17"/>
+        <v>0,263393611744589, 0,366460677209862, 0,238996093832519, 0,0969839221349352, 0,027408499733786, 0,005720034727051, 0,00091188959416755, 0,000113278210455596, 1,10815640663083E-05, 8,56546014787117E-07, 5,2137583508781E-08, 2,47292886207657E-09, 8,95988718143687E-11, 2,39729422914699E-12, 4,46700788039809E-14</v>
+      </c>
+      <c r="Q20" t="str">
+        <f t="shared" si="18"/>
+        <v>0,263393611744589, 0,366460677209862, 0,238996093832519, 0,0969839221349352, 0,027408499733786, 0,005720034727051, 0,00091188959416755, 0,000113278210455596, 1,10815640663083E-05, 8,56546014787117E-07, 5,2137583508781E-08, 2,47292886207657E-09, 8,95988718143687E-11, 2,39729422914699E-12, 4,46700788039809E-14, 5,17913957147607E-16</v>
+      </c>
+      <c r="R20" t="str">
+        <f t="shared" si="19"/>
+        <v>0,263393611744589, 0,366460677209862, 0,238996093832519, 0,0969839221349352, 0,027408499733786, 0,005720034727051, 0,00091188959416755, 0,000113278210455596, 1,10815640663083E-05, 8,56546014787117E-07, 5,2137583508781E-08, 2,47292886207657E-09, 8,95988718143687E-11, 2,39729422914699E-12, 4,46700788039809E-14, 5,17913957147607E-16, 2,81474976710655E-18</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B21">
-        <f>SUM(B15:B18) - 4*B19</f>
-        <v>18.221061439076006</v>
-      </c>
-      <c r="C21">
-        <f t="shared" ref="C21:Q21" si="15">SUM(C15:C18) - 4*C19</f>
-        <v>11.990034690350752</v>
-      </c>
-      <c r="D21">
+        <f t="shared" si="20"/>
+        <v>1.5258789062500007E-5</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="21"/>
+        <v>0,0000152587890625, 0,000244140625</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="5"/>
+        <v>0,0000152587890625, 0,000244140625, 0,0018310546875</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="6"/>
+        <v>0,0000152587890625, 0,000244140625, 0,0018310546875, 0,00854492187499999</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="7"/>
+        <v>0,0000152587890625, 0,000244140625, 0,0018310546875, 0,00854492187499999, 0,02777099609375</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="8"/>
+        <v>0,0000152587890625, 0,000244140625, 0,0018310546875, 0,00854492187499999, 0,02777099609375, 0,066650390625</v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="9"/>
+        <v>0,0000152587890625, 0,000244140625, 0,0018310546875, 0,00854492187499999, 0,02777099609375, 0,066650390625, 0,1221923828125</v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" si="10"/>
+        <v>0,0000152587890625, 0,000244140625, 0,0018310546875, 0,00854492187499999, 0,02777099609375, 0,066650390625, 0,1221923828125, 0,174560546875</v>
+      </c>
+      <c r="J21" t="str">
+        <f t="shared" si="11"/>
+        <v>0,0000152587890625, 0,000244140625, 0,0018310546875, 0,00854492187499999, 0,02777099609375, 0,066650390625, 0,1221923828125, 0,174560546875, 0,196380615234375</v>
+      </c>
+      <c r="K21" t="str">
+        <f t="shared" si="12"/>
+        <v>0,0000152587890625, 0,000244140625, 0,0018310546875, 0,00854492187499999, 0,02777099609375, 0,066650390625, 0,1221923828125, 0,174560546875, 0,196380615234375, 0,174560546875</v>
+      </c>
+      <c r="L21" t="str">
+        <f t="shared" si="13"/>
+        <v>0,0000152587890625, 0,000244140625, 0,0018310546875, 0,00854492187499999, 0,02777099609375, 0,066650390625, 0,1221923828125, 0,174560546875, 0,196380615234375, 0,174560546875, 0,1221923828125</v>
+      </c>
+      <c r="M21" t="str">
+        <f t="shared" si="14"/>
+        <v>0,0000152587890625, 0,000244140625, 0,0018310546875, 0,00854492187499999, 0,02777099609375, 0,066650390625, 0,1221923828125, 0,174560546875, 0,196380615234375, 0,174560546875, 0,1221923828125, 0,066650390625</v>
+      </c>
+      <c r="N21" t="str">
         <f t="shared" si="15"/>
-        <v>5.7590079416255016</v>
-      </c>
-      <c r="E21">
-        <f t="shared" si="15"/>
-        <v>-0.47201880709974731</v>
-      </c>
-      <c r="F21">
-        <f t="shared" si="15"/>
-        <v>-6.7030455558250006</v>
-      </c>
-      <c r="G21">
-        <f t="shared" si="15"/>
-        <v>-12.934072304550252</v>
-      </c>
-      <c r="H21">
-        <f t="shared" si="15"/>
-        <v>-19.165099053275505</v>
-      </c>
-      <c r="I21">
-        <f t="shared" si="15"/>
-        <v>-25.396125802000753</v>
-      </c>
-      <c r="J21">
-        <f t="shared" si="15"/>
-        <v>-31.627152550726009</v>
-      </c>
-      <c r="K21">
-        <f t="shared" si="15"/>
-        <v>-37.858179299451258</v>
-      </c>
-      <c r="L21">
-        <f t="shared" si="15"/>
-        <v>-44.089206048176514</v>
-      </c>
-      <c r="M21">
-        <f t="shared" si="15"/>
-        <v>-50.320232796901763</v>
-      </c>
-      <c r="N21">
-        <f t="shared" si="15"/>
-        <v>-56.551259545627012</v>
-      </c>
-      <c r="O21">
-        <f t="shared" si="15"/>
-        <v>-62.782286294352275</v>
-      </c>
-      <c r="P21">
-        <f t="shared" si="15"/>
-        <v>-69.013313043077517</v>
-      </c>
-      <c r="Q21">
-        <f t="shared" si="15"/>
-        <v>-75.244339791802759</v>
-      </c>
-      <c r="R21">
-        <f t="shared" ref="R21" si="16">SUM(R15:R18) - 4*R19</f>
-        <v>-81.475366540528015</v>
+        <v>0,0000152587890625, 0,000244140625, 0,0018310546875, 0,00854492187499999, 0,02777099609375, 0,066650390625, 0,1221923828125, 0,174560546875, 0,196380615234375, 0,174560546875, 0,1221923828125, 0,066650390625, 0,02777099609375</v>
+      </c>
+      <c r="O21" t="str">
+        <f t="shared" si="16"/>
+        <v>0,0000152587890625, 0,000244140625, 0,0018310546875, 0,00854492187499999, 0,02777099609375, 0,066650390625, 0,1221923828125, 0,174560546875, 0,196380615234375, 0,174560546875, 0,1221923828125, 0,066650390625, 0,02777099609375, 0,00854492187499999</v>
+      </c>
+      <c r="P21" t="str">
+        <f t="shared" si="17"/>
+        <v>0,0000152587890625, 0,000244140625, 0,0018310546875, 0,00854492187499999, 0,02777099609375, 0,066650390625, 0,1221923828125, 0,174560546875, 0,196380615234375, 0,174560546875, 0,1221923828125, 0,066650390625, 0,02777099609375, 0,00854492187499999, 0,0018310546875</v>
+      </c>
+      <c r="Q21" t="str">
+        <f t="shared" si="18"/>
+        <v>0,0000152587890625, 0,000244140625, 0,0018310546875, 0,00854492187499999, 0,02777099609375, 0,066650390625, 0,1221923828125, 0,174560546875, 0,196380615234375, 0,174560546875, 0,1221923828125, 0,066650390625, 0,02777099609375, 0,00854492187499999, 0,0018310546875, 0,000244140625</v>
+      </c>
+      <c r="R21" t="str">
+        <f t="shared" si="19"/>
+        <v>0,0000152587890625, 0,000244140625, 0,0018310546875, 0,00854492187499999, 0,02777099609375, 0,066650390625, 0,1221923828125, 0,174560546875, 0,196380615234375, 0,174560546875, 0,1221923828125, 0,066650390625, 0,02777099609375, 0,00854492187499999, 0,0018310546875, 0,000244140625, 0,0000152587890625</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
       <c r="B24">
-        <f>B15</f>
+        <f>LOG(B8)</f>
         <v>-6.282152823559474E-2</v>
       </c>
-      <c r="C24" t="str">
-        <f>CONCATENATE(B24,", ",C15)</f>
-        <v>-0,0628215282355947, -0,900532690625621</v>
-      </c>
-      <c r="D24" t="str">
-        <f t="shared" ref="D24:R24" si="17">CONCATENATE(C24,", ",D15)</f>
-        <v>-0,0628215282355947, -0,900532690625621, -2,06730257227987</v>
-      </c>
-      <c r="E24" t="str">
-        <f t="shared" si="17"/>
-        <v>-0,0628215282355947, -0,900532690625621, -2,06730257227987, -3,44012693636725</v>
-      </c>
-      <c r="F24" t="str">
-        <f t="shared" si="17"/>
-        <v>-0,0628215282355947, -0,900532690625621, -2,06730257227987, -3,44012693636725, -4,97007472043432</v>
-      </c>
-      <c r="G24" t="str">
-        <f t="shared" si="17"/>
-        <v>-0,0628215282355947, -0,900532690625621, -2,06730257227987, -3,44012693636725, -4,97007472043432, -6,63169462376867</v>
-      </c>
-      <c r="H24" t="str">
-        <f t="shared" si="17"/>
-        <v>-0,0628215282355947, -0,900532690625621, -2,06730257227987, -3,44012693636725, -4,97007472043432, -6,63169462376867, -8,41028433404004</v>
-      </c>
-      <c r="I24" t="str">
-        <f t="shared" si="17"/>
-        <v>-0,0628215282355947, -0,900532690625621, -2,06730257227987, -3,44012693636725, -4,97007472043432, -6,63169462376867, -8,41028433404004, -10,2972135191002</v>
-      </c>
-      <c r="J24" t="str">
-        <f t="shared" si="17"/>
-        <v>-0,0628215282355947, -0,900532690625621, -2,06730257227987, -3,44012693636725, -4,97007472043432, -6,63169462376867, -8,41028433404004, -10,2972135191002, -12,2878921416988</v>
-      </c>
-      <c r="K24" t="str">
-        <f t="shared" si="17"/>
-        <v>-0,0628215282355947, -0,900532690625621, -2,06730257227987, -3,44012693636725, -4,97007472043432, -6,63169462376867, -8,41028433404004, -10,2972135191002, -12,2878921416988, -14,3808758091921</v>
-      </c>
-      <c r="L24" t="str">
-        <f t="shared" si="17"/>
-        <v>-0,0628215282355947, -0,900532690625621, -2,06730257227987, -3,44012693636725, -4,97007472043432, -6,63169462376867, -8,41028433404004, -10,2972135191002, -12,2878921416988, -14,3808758091921, -16,5776089142238</v>
-      </c>
-      <c r="M24" t="str">
-        <f t="shared" si="17"/>
-        <v>-0,0628215282355947, -0,900532690625621, -2,06730257227987, -3,44012693636725, -4,97007472043432, -6,63169462376867, -8,41028433404004, -10,2972135191002, -12,2878921416988, -14,3808758091921, -16,5776089142238, -18,8826814940444</v>
-      </c>
-      <c r="N24" t="str">
-        <f t="shared" si="17"/>
-        <v>-0,0628215282355947, -0,900532690625621, -2,06730257227987, -3,44012693636725, -4,97007472043432, -6,63169462376867, -8,41028433404004, -10,2972135191002, -12,2878921416988, -14,3808758091921, -16,5776089142238, -18,8826814940444, -21,3047238808019</v>
-      </c>
-      <c r="O24" t="str">
-        <f t="shared" si="17"/>
-        <v>-0,0628215282355947, -0,900532690625621, -2,06730257227987, -3,44012693636725, -4,97007472043432, -6,63169462376867, -8,41028433404004, -10,2972135191002, -12,2878921416988, -14,3808758091921, -16,5776089142238, -18,8826814940444, -21,3047238808019, -23,8584383868268</v>
-      </c>
-      <c r="P24" t="str">
-        <f t="shared" si="17"/>
-        <v>-0,0628215282355947, -0,900532690625621, -2,06730257227987, -3,44012693636725, -4,97007472043432, -6,63169462376867, -8,41028433404004, -10,2972135191002, -12,2878921416988, -14,3808758091921, -16,5776089142238, -18,8826814940444, -21,3047238808019, -23,8584383868268, -26,5692763128313</v>
-      </c>
-      <c r="Q24" t="str">
-        <f t="shared" si="17"/>
-        <v>-0,0628215282355947, -0,900532690625621, -2,06730257227987, -3,44012693636725, -4,97007472043432, -6,63169462376867, -8,41028433404004, -10,2972135191002, -12,2878921416988, -14,3808758091921, -16,5776089142238, -18,8826814940444, -21,3047238808019, -23,8584383868268, -26,5692763128313, -29,4861687212689</v>
-      </c>
-      <c r="R24" t="str">
-        <f t="shared" si="17"/>
-        <v>-0,0628215282355947, -0,900532690625621, -2,06730257227987, -3,44012693636725, -4,97007472043432, -6,63169462376867, -8,41028433404004, -10,2972135191002, -12,2878921416988, -14,3808758091921, -16,5776089142238, -18,8826814940444, -21,3047238808019, -23,8584383868268, -26,5692763128313, -29,4861687212689, -32,7321198489708</v>
+      <c r="C24">
+        <f>LOG(C8)</f>
+        <v>-0.90053269062562058</v>
+      </c>
+      <c r="D24">
+        <f>LOG(D8)</f>
+        <v>-2.0673025722798708</v>
+      </c>
+      <c r="E24">
+        <f>LOG(E8)</f>
+        <v>-3.4401269363672458</v>
+      </c>
+      <c r="F24">
+        <f>LOG(F8)</f>
+        <v>-4.9700747204343214</v>
+      </c>
+      <c r="G24">
+        <f>LOG(G8)</f>
+        <v>-6.6316946237686665</v>
+      </c>
+      <c r="H24">
+        <f>LOG(H8)</f>
+        <v>-8.4102843340400355</v>
+      </c>
+      <c r="I24">
+        <f>LOG(I8)</f>
+        <v>-10.297213519100243</v>
+      </c>
+      <c r="J24">
+        <f>LOG(J8)</f>
+        <v>-12.28789214169881</v>
+      </c>
+      <c r="K24">
+        <f>LOG(K8)</f>
+        <v>-14.380875809192142</v>
+      </c>
+      <c r="L24">
+        <f>LOG(L8)</f>
+        <v>-16.577608914223838</v>
+      </c>
+      <c r="M24">
+        <f>LOG(M8)</f>
+        <v>-18.882681494044366</v>
+      </c>
+      <c r="N24">
+        <f>LOG(N8)</f>
+        <v>-21.304723880801927</v>
+      </c>
+      <c r="O24">
+        <f>LOG(O8)</f>
+        <v>-23.858438386826752</v>
+      </c>
+      <c r="P24">
+        <f>LOG(P8)</f>
+        <v>-26.569276312831274</v>
+      </c>
+      <c r="Q24">
+        <f>LOG(Q8)</f>
+        <v>-29.486168721268925</v>
+      </c>
+      <c r="R24">
+        <f>LOG(R8)</f>
+        <v>-32.732119848970804</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>9</v>
+      </c>
       <c r="B25">
-        <f t="shared" ref="B25:B28" si="18">B16</f>
+        <f>LOG(B9)</f>
         <v>-0.1262161954088053</v>
       </c>
-      <c r="C25" t="str">
-        <f t="shared" ref="C25:R28" si="19">CONCATENATE(B25,", ",C16)</f>
-        <v>-0,126216195408805, -0,658935195436524</v>
-      </c>
-      <c r="D25" t="str">
-        <f t="shared" si="19"/>
-        <v>-0,126216195408805, -0,658935195436524, -1,52071291472847</v>
-      </c>
-      <c r="E25" t="str">
-        <f t="shared" si="19"/>
-        <v>-0,126216195408805, -0,658935195436524, -1,52071291472847, -2,58854511645354</v>
-      </c>
-      <c r="F25" t="str">
-        <f t="shared" si="19"/>
-        <v>-0,126216195408805, -0,658935195436524, -1,52071291472847, -2,58854511645354, -3,81350073815831</v>
-      </c>
-      <c r="G25" t="str">
-        <f t="shared" si="19"/>
-        <v>-0,126216195408805, -0,658935195436524, -1,52071291472847, -2,58854511645354, -3,81350073815831, -5,17012847913034</v>
-      </c>
-      <c r="H25" t="str">
-        <f t="shared" si="19"/>
-        <v>-0,126216195408805, -0,658935195436524, -1,52071291472847, -2,58854511645354, -3,81350073815831, -5,17012847913034, -6,64372602703941</v>
-      </c>
-      <c r="I25" t="str">
-        <f t="shared" si="19"/>
-        <v>-0,126216195408805, -0,658935195436524, -1,52071291472847, -2,58854511645354, -3,81350073815831, -5,17012847913034, -6,64372602703941, -8,2256630497373</v>
-      </c>
-      <c r="J25" t="str">
-        <f t="shared" si="19"/>
-        <v>-0,126216195408805, -0,658935195436524, -1,52071291472847, -2,58854511645354, -3,81350073815831, -5,17012847913034, -6,64372602703941, -8,2256630497373, -9,91134950997357</v>
-      </c>
-      <c r="K25" t="str">
-        <f t="shared" si="19"/>
-        <v>-0,126216195408805, -0,658935195436524, -1,52071291472847, -2,58854511645354, -3,81350073815831, -5,17012847913034, -6,64372602703941, -8,2256630497373, -9,91134950997357, -11,6993410151046</v>
-      </c>
-      <c r="L25" t="str">
-        <f t="shared" si="19"/>
-        <v>-0,126216195408805, -0,658935195436524, -1,52071291472847, -2,58854511645354, -3,81350073815831, -5,17012847913034, -6,64372602703941, -8,2256630497373, -9,91134950997357, -11,6993410151046, -13,591081957774</v>
-      </c>
-      <c r="M25" t="str">
-        <f t="shared" si="19"/>
-        <v>-0,126216195408805, -0,658935195436524, -1,52071291472847, -2,58854511645354, -3,81350073815831, -5,17012847913034, -6,64372602703941, -8,2256630497373, -9,91134950997357, -11,6993410151046, -13,591081957774, -15,5911623752322</v>
-      </c>
-      <c r="N25" t="str">
-        <f t="shared" si="19"/>
-        <v>-0,126216195408805, -0,658935195436524, -1,52071291472847, -2,58854511645354, -3,81350073815831, -5,17012847913034, -6,64372602703941, -8,2256630497373, -9,91134950997357, -11,6993410151046, -13,591081957774, -15,5911623752322, -17,7082125996275</v>
-      </c>
-      <c r="O25" t="str">
-        <f t="shared" si="19"/>
-        <v>-0,126216195408805, -0,658935195436524, -1,52071291472847, -2,58854511645354, -3,81350073815831, -5,17012847913034, -6,64372602703941, -8,2256630497373, -9,91134950997357, -11,6993410151046, -13,591081957774, -15,5911623752322, -17,7082125996275, -19,95693494329</v>
-      </c>
-      <c r="P25" t="str">
-        <f t="shared" si="19"/>
-        <v>-0,126216195408805, -0,658935195436524, -1,52071291472847, -2,58854511645354, -3,81350073815831, -5,17012847913034, -6,64372602703941, -8,2256630497373, -9,91134950997357, -11,6993410151046, -13,591081957774, -15,5911623752322, -17,7082125996275, -19,95693494329, -22,3627807069322</v>
-      </c>
-      <c r="Q25" t="str">
-        <f t="shared" si="19"/>
-        <v>-0,126216195408805, -0,658935195436524, -1,52071291472847, -2,58854511645354, -3,81350073815831, -5,17012847913034, -6,64372602703941, -8,2256630497373, -9,91134950997357, -11,6993410151046, -13,591081957774, -15,5911623752322, -17,7082125996275, -19,95693494329, -22,3627807069322, -24,9746809530075</v>
-      </c>
-      <c r="R25" t="str">
-        <f t="shared" si="19"/>
-        <v>-0,126216195408805, -0,658935195436524, -1,52071291472847, -2,58854511645354, -3,81350073815831, -5,17012847913034, -6,64372602703941, -8,2256630497373, -9,91134950997357, -11,6993410151046, -13,591081957774, -15,5911623752322, -17,7082125996275, -19,95693494329, -22,3627807069322, -24,9746809530075, -27,9156399183471</v>
+      <c r="C25">
+        <f>LOG(C9)</f>
+        <v>-0.65893519543652423</v>
+      </c>
+      <c r="D25">
+        <f>LOG(D9)</f>
+        <v>-1.5207129147284679</v>
+      </c>
+      <c r="E25">
+        <f>LOG(E9)</f>
+        <v>-2.5885451164535356</v>
+      </c>
+      <c r="F25">
+        <f>LOG(F9)</f>
+        <v>-3.8135007381583055</v>
+      </c>
+      <c r="G25">
+        <f>LOG(G9)</f>
+        <v>-5.1701284791303426</v>
+      </c>
+      <c r="H25">
+        <f>LOG(H9)</f>
+        <v>-6.6437260270394054</v>
+      </c>
+      <c r="I25">
+        <f>LOG(I9)</f>
+        <v>-8.2256630497373049</v>
+      </c>
+      <c r="J25">
+        <f>LOG(J9)</f>
+        <v>-9.9113495099735669</v>
+      </c>
+      <c r="K25">
+        <f>LOG(K9)</f>
+        <v>-11.699341015104592</v>
+      </c>
+      <c r="L25">
+        <f>LOG(L9)</f>
+        <v>-13.591081957773978</v>
+      </c>
+      <c r="M25">
+        <f>LOG(M9)</f>
+        <v>-15.591162375232207</v>
+      </c>
+      <c r="N25">
+        <f>LOG(N9)</f>
+        <v>-17.708212599627451</v>
+      </c>
+      <c r="O25">
+        <f>LOG(O9)</f>
+        <v>-19.956934943289976</v>
+      </c>
+      <c r="P25">
+        <f>LOG(P9)</f>
+        <v>-22.362780706932195</v>
+      </c>
+      <c r="Q25">
+        <f>LOG(Q9)</f>
+        <v>-24.974680953007535</v>
+      </c>
+      <c r="R25">
+        <f>LOG(R9)</f>
+        <v>-27.915639918347104</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>8</v>
+      </c>
       <c r="B26">
-        <f t="shared" si="18"/>
+        <f>LOG(B10)</f>
         <v>-0.27642579730327427</v>
       </c>
-      <c r="C26" t="str">
-        <f t="shared" si="19"/>
-        <v>-0,276425797303274, -0,463964595289396</v>
-      </c>
-      <c r="D26" t="str">
-        <f t="shared" si="19"/>
-        <v>-0,276425797303274, -0,463964595289396, -0,980562112539742</v>
-      </c>
-      <c r="E26" t="str">
-        <f t="shared" si="19"/>
-        <v>-0,276425797303274, -0,463964595289396, -0,980562112539742, -1,70321411222321</v>
-      </c>
-      <c r="F26" t="str">
-        <f t="shared" si="19"/>
-        <v>-0,276425797303274, -0,463964595289396, -0,980562112539742, -1,70321411222321, -2,58298953188638</v>
-      </c>
-      <c r="G26" t="str">
-        <f t="shared" si="19"/>
-        <v>-0,276425797303274, -0,463964595289396, -0,980562112539742, -1,70321411222321, -2,58298953188638, -3,59443707081682</v>
-      </c>
-      <c r="H26" t="str">
-        <f t="shared" si="19"/>
-        <v>-0,276425797303274, -0,463964595289396, -0,980562112539742, -1,70321411222321, -2,58298953188638, -3,59443707081682, -4,72285441668429</v>
-      </c>
-      <c r="I26" t="str">
-        <f t="shared" si="19"/>
-        <v>-0,276425797303274, -0,463964595289396, -0,980562112539742, -1,70321411222321, -2,58298953188638, -3,59443707081682, -4,72285441668429, -5,95961123734059</v>
-      </c>
-      <c r="J26" t="str">
-        <f t="shared" si="19"/>
-        <v>-0,276425797303274, -0,463964595289396, -0,980562112539742, -1,70321411222321, -2,58298953188638, -3,59443707081682, -4,72285441668429, -5,95961123734059, -7,30011749553526</v>
-      </c>
-      <c r="K26" t="str">
-        <f t="shared" si="19"/>
-        <v>-0,276425797303274, -0,463964595289396, -0,980562112539742, -1,70321411222321, -2,58298953188638, -3,59443707081682, -4,72285441668429, -5,95961123734059, -7,30011749553526, -8,74292879862468</v>
-      </c>
-      <c r="L26" t="str">
-        <f t="shared" si="19"/>
-        <v>-0,276425797303274, -0,463964595289396, -0,980562112539742, -1,70321411222321, -2,58298953188638, -3,59443707081682, -4,72285441668429, -5,95961123734059, -7,30011749553526, -8,74292879862468, -10,2894895392525</v>
-      </c>
-      <c r="M26" t="str">
-        <f t="shared" si="19"/>
-        <v>-0,276425797303274, -0,463964595289396, -0,980562112539742, -1,70321411222321, -2,58298953188638, -3,59443707081682, -4,72285441668429, -5,95961123734059, -7,30011749553526, -8,74292879862468, -10,2894895392525, -11,9443897546691</v>
-      </c>
-      <c r="N26" t="str">
-        <f t="shared" si="19"/>
-        <v>-0,276425797303274, -0,463964595289396, -0,980562112539742, -1,70321411222321, -2,58298953188638, -3,59443707081682, -4,72285441668429, -5,95961123734059, -7,30011749553526, -8,74292879862468, -10,2894895392525, -11,9443897546691, -13,7162597770228</v>
-      </c>
-      <c r="O26" t="str">
-        <f t="shared" si="19"/>
-        <v>-0,276425797303274, -0,463964595289396, -0,980562112539742, -1,70321411222321, -2,58298953188638, -3,59443707081682, -4,72285441668429, -5,95961123734059, -7,30011749553526, -8,74292879862468, -10,2894895392525, -11,9443897546691, -13,7162597770228, -15,6198019186437</v>
-      </c>
-      <c r="P26" t="str">
-        <f t="shared" si="19"/>
-        <v>-0,276425797303274, -0,463964595289396, -0,980562112539742, -1,70321411222321, -2,58298953188638, -3,59443707081682, -4,72285441668429, -5,95961123734059, -7,30011749553526, -8,74292879862468, -10,2894895392525, -11,9443897546691, -13,7162597770228, -15,6198019186437, -17,6804674802443</v>
-      </c>
-      <c r="Q26" t="str">
-        <f t="shared" si="19"/>
-        <v>-0,276425797303274, -0,463964595289396, -0,980562112539742, -1,70321411222321, -2,58298953188638, -3,59443707081682, -4,72285441668429, -5,95961123734059, -7,30011749553526, -8,74292879862468, -10,2894895392525, -11,9443897546691, -13,7162597770228, -15,6198019186437, -17,6804674802443, -19,947187524278</v>
-      </c>
-      <c r="R26" t="str">
-        <f t="shared" si="19"/>
-        <v>-0,276425797303274, -0,463964595289396, -0,980562112539742, -1,70321411222321, -2,58298953188638, -3,59443707081682, -4,72285441668429, -5,95961123734059, -7,30011749553526, -8,74292879862468, -10,2894895392525, -11,9443897546691, -13,7162597770228, -15,6198019186437, -17,6804674802443, -19,947187524278, -22,542966287576</v>
+      <c r="C26">
+        <f>LOG(C10)</f>
+        <v>-0.46396459528939565</v>
+      </c>
+      <c r="D26">
+        <f>LOG(D10)</f>
+        <v>-0.98056211253974168</v>
+      </c>
+      <c r="E26">
+        <f>LOG(E10)</f>
+        <v>-1.7032141122232123</v>
+      </c>
+      <c r="F26">
+        <f>LOG(F10)</f>
+        <v>-2.5829895318863842</v>
+      </c>
+      <c r="G26">
+        <f>LOG(G10)</f>
+        <v>-3.5944370708168241</v>
+      </c>
+      <c r="H26">
+        <f>LOG(H10)</f>
+        <v>-4.7228544166842878</v>
+      </c>
+      <c r="I26">
+        <f>LOG(I10)</f>
+        <v>-5.9596112373405914</v>
+      </c>
+      <c r="J26">
+        <f>LOG(J10)</f>
+        <v>-7.3001174955352575</v>
+      </c>
+      <c r="K26">
+        <f>LOG(K10)</f>
+        <v>-8.7429287986246838</v>
+      </c>
+      <c r="L26">
+        <f>LOG(L10)</f>
+        <v>-10.289489539252472</v>
+      </c>
+      <c r="M26">
+        <f>LOG(M10)</f>
+        <v>-11.944389754669103</v>
+      </c>
+      <c r="N26">
+        <f>LOG(N10)</f>
+        <v>-13.716259777022753</v>
+      </c>
+      <c r="O26">
+        <f>LOG(O10)</f>
+        <v>-15.619801918643676</v>
+      </c>
+      <c r="P26">
+        <f>LOG(P10)</f>
+        <v>-17.680467480244296</v>
+      </c>
+      <c r="Q26">
+        <f>LOG(Q10)</f>
+        <v>-19.947187524278043</v>
+      </c>
+      <c r="R26">
+        <f>LOG(R10)</f>
+        <v>-22.542966287576011</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>8</v>
+      </c>
       <c r="B27">
-        <f t="shared" si="18"/>
+        <f>LOG(B11)</f>
         <v>-0.57939476247111577</v>
       </c>
-      <c r="C27" t="str">
-        <f t="shared" si="19"/>
-        <v>-0,579394762471116, -0,435972620168803</v>
-      </c>
-      <c r="D27" t="str">
-        <f t="shared" si="19"/>
-        <v>-0,579394762471116, -0,435972620168803, -0,621609197130714</v>
-      </c>
-      <c r="E27" t="str">
-        <f t="shared" si="19"/>
-        <v>-0,579394762471116, -0,435972620168803, -0,621609197130714, -1,01330025652575</v>
-      </c>
-      <c r="F27" t="str">
-        <f t="shared" si="19"/>
-        <v>-0,579394762471116, -0,435972620168803, -0,621609197130714, -1,01330025652575, -1,56211473590049</v>
-      </c>
-      <c r="G27" t="str">
-        <f t="shared" si="19"/>
-        <v>-0,579394762471116, -0,435972620168803, -0,621609197130714, -1,01330025652575, -1,56211473590049, -2,24260133454249</v>
-      </c>
-      <c r="H27" t="str">
-        <f t="shared" si="19"/>
-        <v>-0,579394762471116, -0,435972620168803, -0,621609197130714, -1,01330025652575, -1,56211473590049, -2,24260133454249, -3,04005774012152</v>
-      </c>
-      <c r="I27" t="str">
-        <f t="shared" si="19"/>
-        <v>-0,579394762471116, -0,435972620168803, -0,621609197130714, -1,01330025652575, -1,56211473590049, -2,24260133454249, -3,04005774012152, -3,94585362048939</v>
-      </c>
-      <c r="J27" t="str">
-        <f t="shared" si="19"/>
-        <v>-0,579394762471116, -0,435972620168803, -0,621609197130714, -1,01330025652575, -1,56211473590049, -2,24260133454249, -3,04005774012152, -3,94585362048939, -4,95539893839562</v>
-      </c>
-      <c r="K27" t="str">
-        <f t="shared" si="19"/>
-        <v>-0,579394762471116, -0,435972620168803, -0,621609197130714, -1,01330025652575, -1,56211473590049, -2,24260133454249, -3,04005774012152, -3,94585362048939, -4,95539893839562, -6,06724930119662</v>
-      </c>
-      <c r="L27" t="str">
-        <f t="shared" si="19"/>
-        <v>-0,579394762471116, -0,435972620168803, -0,621609197130714, -1,01330025652575, -1,56211473590049, -2,24260133454249, -3,04005774012152, -3,94585362048939, -4,95539893839562, -6,06724930119662, -7,28284910153597</v>
-      </c>
-      <c r="M27" t="str">
-        <f t="shared" si="19"/>
-        <v>-0,579394762471116, -0,435972620168803, -0,621609197130714, -1,01330025652575, -1,56211473590049, -2,24260133454249, -3,04005774012152, -3,94585362048939, -4,95539893839562, -6,06724930119662, -7,28284910153597, -8,60678837666416</v>
-      </c>
-      <c r="N27" t="str">
-        <f t="shared" si="19"/>
-        <v>-0,579394762471116, -0,435972620168803, -0,621609197130714, -1,01330025652575, -1,56211473590049, -2,24260133454249, -3,04005774012152, -3,94585362048939, -4,95539893839562, -6,06724930119662, -7,28284910153597, -8,60678837666416, -10,0476974587294</v>
-      </c>
-      <c r="O27" t="str">
-        <f t="shared" si="19"/>
-        <v>-0,579394762471116, -0,435972620168803, -0,621609197130714, -1,01330025652575, -1,56211473590049, -2,24260133454249, -3,04005774012152, -3,94585362048939, -4,95539893839562, -6,06724930119662, -7,28284910153597, -8,60678837666416, -10,0476974587294, -11,6202786600619</v>
-      </c>
-      <c r="P27" t="str">
-        <f t="shared" si="19"/>
-        <v>-0,579394762471116, -0,435972620168803, -0,621609197130714, -1,01330025652575, -1,56211473590049, -2,24260133454249, -3,04005774012152, -3,94585362048939, -4,95539893839562, -6,06724930119662, -7,28284910153597, -8,60678837666416, -10,0476974587294, -11,6202786600619, -13,3499832813741</v>
-      </c>
-      <c r="Q27" t="str">
-        <f t="shared" si="19"/>
-        <v>-0,579394762471116, -0,435972620168803, -0,621609197130714, -1,01330025652575, -1,56211473590049, -2,24260133454249, -3,04005774012152, -3,94585362048939, -4,95539893839562, -6,06724930119662, -7,28284910153597, -8,60678837666416, -10,0476974587294, -11,6202786600619, -13,3499832813741, -15,2857423851194</v>
-      </c>
-      <c r="R27" t="str">
-        <f t="shared" si="19"/>
-        <v>-0,579394762471116, -0,435972620168803, -0,621609197130714, -1,01330025652575, -1,56211473590049, -2,24260133454249, -3,04005774012152, -3,94585362048939, -4,95539893839562, -6,06724930119662, -7,28284910153597, -8,60678837666416, -10,0476974587294, -11,6202786600619, -13,3499832813741, -15,2857423851194, -17,5505602081289</v>
+      <c r="C27">
+        <f>LOG(C11)</f>
+        <v>-0.43597262016880262</v>
+      </c>
+      <c r="D27">
+        <f>LOG(D11)</f>
+        <v>-0.62160919713071427</v>
+      </c>
+      <c r="E27">
+        <f>LOG(E11)</f>
+        <v>-1.0133002565257505</v>
+      </c>
+      <c r="F27">
+        <f>LOG(F11)</f>
+        <v>-1.5621147359004877</v>
+      </c>
+      <c r="G27">
+        <f>LOG(G11)</f>
+        <v>-2.2426013345424933</v>
+      </c>
+      <c r="H27">
+        <f>LOG(H11)</f>
+        <v>-3.0400577401215236</v>
+      </c>
+      <c r="I27">
+        <f>LOG(I11)</f>
+        <v>-3.9458536204893924</v>
+      </c>
+      <c r="J27">
+        <f>LOG(J11)</f>
+        <v>-4.9553989383956232</v>
+      </c>
+      <c r="K27">
+        <f>LOG(K11)</f>
+        <v>-6.0672493011966155</v>
+      </c>
+      <c r="L27">
+        <f>LOG(L11)</f>
+        <v>-7.2828491015359713</v>
+      </c>
+      <c r="M27">
+        <f>LOG(M11)</f>
+        <v>-8.6067883766641646</v>
+      </c>
+      <c r="N27">
+        <f>LOG(N11)</f>
+        <v>-10.047697458729381</v>
+      </c>
+      <c r="O27">
+        <f>LOG(O11)</f>
+        <v>-11.620278660061865</v>
+      </c>
+      <c r="P27">
+        <f>LOG(P11)</f>
+        <v>-13.349983281374056</v>
+      </c>
+      <c r="Q27">
+        <f>LOG(Q11)</f>
+        <v>-15.285742385119367</v>
+      </c>
+      <c r="R27">
+        <f>LOG(R11)</f>
+        <v>-17.550560208128903</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>10</v>
+      </c>
       <c r="B28">
-        <f t="shared" si="18"/>
+        <f>LOG(B12)</f>
         <v>-4.8164799306236992</v>
       </c>
-      <c r="C28" t="str">
-        <f t="shared" si="19"/>
+      <c r="C28">
+        <f>LOG(C12)</f>
+        <v>-3.6123599479677737</v>
+      </c>
+      <c r="D28">
+        <f>LOG(D12)</f>
+        <v>-2.7372986845760741</v>
+      </c>
+      <c r="E28">
+        <f>LOG(E12)</f>
+        <v>-2.0682919036174989</v>
+      </c>
+      <c r="F28">
+        <f>LOG(F12)</f>
+        <v>-1.5564085426386243</v>
+      </c>
+      <c r="G28">
+        <f>LOG(G12)</f>
+        <v>-1.1761973009270184</v>
+      </c>
+      <c r="H28">
+        <f>LOG(H12)</f>
+        <v>-0.91295586615243696</v>
+      </c>
+      <c r="I28">
+        <f>LOG(I12)</f>
+        <v>-0.75805390616669377</v>
+      </c>
+      <c r="J28">
+        <f>LOG(J12)</f>
+        <v>-0.70690138371931244</v>
+      </c>
+      <c r="K28">
+        <f>LOG(K12)</f>
+        <v>-0.75805390616669377</v>
+      </c>
+      <c r="L28">
+        <f>LOG(L12)</f>
+        <v>-0.91295586615243696</v>
+      </c>
+      <c r="M28">
+        <f>LOG(M12)</f>
+        <v>-1.1761973009270184</v>
+      </c>
+      <c r="N28">
+        <f>LOG(N12)</f>
+        <v>-1.5564085426386243</v>
+      </c>
+      <c r="O28">
+        <f>LOG(O12)</f>
+        <v>-2.0682919036174994</v>
+      </c>
+      <c r="P28">
+        <f>LOG(P12)</f>
+        <v>-2.7372986845760741</v>
+      </c>
+      <c r="Q28">
+        <f>LOG(Q12)</f>
+        <v>-3.6123599479677737</v>
+      </c>
+      <c r="R28">
+        <f>LOG(R12)</f>
+        <v>-4.8164799306236992</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <f>SUM(B24:B27) - 4*B28</f>
+        <v>18.221061439076006</v>
+      </c>
+      <c r="C30">
+        <f t="shared" ref="C30:Q30" si="22">SUM(C24:C27) - 4*C28</f>
+        <v>11.990034690350752</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="22"/>
+        <v>5.7590079416255016</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="22"/>
+        <v>-0.47201880709974731</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="22"/>
+        <v>-6.7030455558250006</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="22"/>
+        <v>-12.934072304550252</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="22"/>
+        <v>-19.165099053275505</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="22"/>
+        <v>-25.396125802000753</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="22"/>
+        <v>-31.627152550726009</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="22"/>
+        <v>-37.858179299451258</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="22"/>
+        <v>-44.089206048176514</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="22"/>
+        <v>-50.320232796901763</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="22"/>
+        <v>-56.551259545627012</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="22"/>
+        <v>-62.782286294352275</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="22"/>
+        <v>-69.013313043077517</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" si="22"/>
+        <v>-75.244339791802759</v>
+      </c>
+      <c r="R30">
+        <f t="shared" ref="R30" si="23">SUM(R24:R27) - 4*R28</f>
+        <v>-81.475366540528015</v>
+      </c>
+    </row>
+    <row r="33" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <f>B24</f>
+        <v>-6.282152823559474E-2</v>
+      </c>
+      <c r="C33" t="str">
+        <f>CONCATENATE(B33,", ",C24)</f>
+        <v>-0,0628215282355947, -0,900532690625621</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" ref="D33:R33" si="24">CONCATENATE(C33,", ",D24)</f>
+        <v>-0,0628215282355947, -0,900532690625621, -2,06730257227987</v>
+      </c>
+      <c r="E33" t="str">
+        <f t="shared" si="24"/>
+        <v>-0,0628215282355947, -0,900532690625621, -2,06730257227987, -3,44012693636725</v>
+      </c>
+      <c r="F33" t="str">
+        <f t="shared" si="24"/>
+        <v>-0,0628215282355947, -0,900532690625621, -2,06730257227987, -3,44012693636725, -4,97007472043432</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="24"/>
+        <v>-0,0628215282355947, -0,900532690625621, -2,06730257227987, -3,44012693636725, -4,97007472043432, -6,63169462376867</v>
+      </c>
+      <c r="H33" t="str">
+        <f t="shared" si="24"/>
+        <v>-0,0628215282355947, -0,900532690625621, -2,06730257227987, -3,44012693636725, -4,97007472043432, -6,63169462376867, -8,41028433404004</v>
+      </c>
+      <c r="I33" t="str">
+        <f t="shared" si="24"/>
+        <v>-0,0628215282355947, -0,900532690625621, -2,06730257227987, -3,44012693636725, -4,97007472043432, -6,63169462376867, -8,41028433404004, -10,2972135191002</v>
+      </c>
+      <c r="J33" t="str">
+        <f t="shared" si="24"/>
+        <v>-0,0628215282355947, -0,900532690625621, -2,06730257227987, -3,44012693636725, -4,97007472043432, -6,63169462376867, -8,41028433404004, -10,2972135191002, -12,2878921416988</v>
+      </c>
+      <c r="K33" t="str">
+        <f t="shared" si="24"/>
+        <v>-0,0628215282355947, -0,900532690625621, -2,06730257227987, -3,44012693636725, -4,97007472043432, -6,63169462376867, -8,41028433404004, -10,2972135191002, -12,2878921416988, -14,3808758091921</v>
+      </c>
+      <c r="L33" t="str">
+        <f t="shared" si="24"/>
+        <v>-0,0628215282355947, -0,900532690625621, -2,06730257227987, -3,44012693636725, -4,97007472043432, -6,63169462376867, -8,41028433404004, -10,2972135191002, -12,2878921416988, -14,3808758091921, -16,5776089142238</v>
+      </c>
+      <c r="M33" t="str">
+        <f t="shared" si="24"/>
+        <v>-0,0628215282355947, -0,900532690625621, -2,06730257227987, -3,44012693636725, -4,97007472043432, -6,63169462376867, -8,41028433404004, -10,2972135191002, -12,2878921416988, -14,3808758091921, -16,5776089142238, -18,8826814940444</v>
+      </c>
+      <c r="N33" t="str">
+        <f t="shared" si="24"/>
+        <v>-0,0628215282355947, -0,900532690625621, -2,06730257227987, -3,44012693636725, -4,97007472043432, -6,63169462376867, -8,41028433404004, -10,2972135191002, -12,2878921416988, -14,3808758091921, -16,5776089142238, -18,8826814940444, -21,3047238808019</v>
+      </c>
+      <c r="O33" t="str">
+        <f t="shared" si="24"/>
+        <v>-0,0628215282355947, -0,900532690625621, -2,06730257227987, -3,44012693636725, -4,97007472043432, -6,63169462376867, -8,41028433404004, -10,2972135191002, -12,2878921416988, -14,3808758091921, -16,5776089142238, -18,8826814940444, -21,3047238808019, -23,8584383868268</v>
+      </c>
+      <c r="P33" t="str">
+        <f t="shared" si="24"/>
+        <v>-0,0628215282355947, -0,900532690625621, -2,06730257227987, -3,44012693636725, -4,97007472043432, -6,63169462376867, -8,41028433404004, -10,2972135191002, -12,2878921416988, -14,3808758091921, -16,5776089142238, -18,8826814940444, -21,3047238808019, -23,8584383868268, -26,5692763128313</v>
+      </c>
+      <c r="Q33" t="str">
+        <f t="shared" si="24"/>
+        <v>-0,0628215282355947, -0,900532690625621, -2,06730257227987, -3,44012693636725, -4,97007472043432, -6,63169462376867, -8,41028433404004, -10,2972135191002, -12,2878921416988, -14,3808758091921, -16,5776089142238, -18,8826814940444, -21,3047238808019, -23,8584383868268, -26,5692763128313, -29,4861687212689</v>
+      </c>
+      <c r="R33" t="str">
+        <f t="shared" si="24"/>
+        <v>-0,0628215282355947, -0,900532690625621, -2,06730257227987, -3,44012693636725, -4,97007472043432, -6,63169462376867, -8,41028433404004, -10,2972135191002, -12,2878921416988, -14,3808758091921, -16,5776089142238, -18,8826814940444, -21,3047238808019, -23,8584383868268, -26,5692763128313, -29,4861687212689, -32,7321198489708</v>
+      </c>
+    </row>
+    <row r="34" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <f t="shared" ref="B34:B37" si="25">B25</f>
+        <v>-0.1262161954088053</v>
+      </c>
+      <c r="C34" t="str">
+        <f t="shared" ref="C34:R37" si="26">CONCATENATE(B34,", ",C25)</f>
+        <v>-0,126216195408805, -0,658935195436524</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="26"/>
+        <v>-0,126216195408805, -0,658935195436524, -1,52071291472847</v>
+      </c>
+      <c r="E34" t="str">
+        <f t="shared" si="26"/>
+        <v>-0,126216195408805, -0,658935195436524, -1,52071291472847, -2,58854511645354</v>
+      </c>
+      <c r="F34" t="str">
+        <f t="shared" si="26"/>
+        <v>-0,126216195408805, -0,658935195436524, -1,52071291472847, -2,58854511645354, -3,81350073815831</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" si="26"/>
+        <v>-0,126216195408805, -0,658935195436524, -1,52071291472847, -2,58854511645354, -3,81350073815831, -5,17012847913034</v>
+      </c>
+      <c r="H34" t="str">
+        <f t="shared" si="26"/>
+        <v>-0,126216195408805, -0,658935195436524, -1,52071291472847, -2,58854511645354, -3,81350073815831, -5,17012847913034, -6,64372602703941</v>
+      </c>
+      <c r="I34" t="str">
+        <f t="shared" si="26"/>
+        <v>-0,126216195408805, -0,658935195436524, -1,52071291472847, -2,58854511645354, -3,81350073815831, -5,17012847913034, -6,64372602703941, -8,2256630497373</v>
+      </c>
+      <c r="J34" t="str">
+        <f t="shared" si="26"/>
+        <v>-0,126216195408805, -0,658935195436524, -1,52071291472847, -2,58854511645354, -3,81350073815831, -5,17012847913034, -6,64372602703941, -8,2256630497373, -9,91134950997357</v>
+      </c>
+      <c r="K34" t="str">
+        <f t="shared" si="26"/>
+        <v>-0,126216195408805, -0,658935195436524, -1,52071291472847, -2,58854511645354, -3,81350073815831, -5,17012847913034, -6,64372602703941, -8,2256630497373, -9,91134950997357, -11,6993410151046</v>
+      </c>
+      <c r="L34" t="str">
+        <f t="shared" si="26"/>
+        <v>-0,126216195408805, -0,658935195436524, -1,52071291472847, -2,58854511645354, -3,81350073815831, -5,17012847913034, -6,64372602703941, -8,2256630497373, -9,91134950997357, -11,6993410151046, -13,591081957774</v>
+      </c>
+      <c r="M34" t="str">
+        <f t="shared" si="26"/>
+        <v>-0,126216195408805, -0,658935195436524, -1,52071291472847, -2,58854511645354, -3,81350073815831, -5,17012847913034, -6,64372602703941, -8,2256630497373, -9,91134950997357, -11,6993410151046, -13,591081957774, -15,5911623752322</v>
+      </c>
+      <c r="N34" t="str">
+        <f t="shared" si="26"/>
+        <v>-0,126216195408805, -0,658935195436524, -1,52071291472847, -2,58854511645354, -3,81350073815831, -5,17012847913034, -6,64372602703941, -8,2256630497373, -9,91134950997357, -11,6993410151046, -13,591081957774, -15,5911623752322, -17,7082125996275</v>
+      </c>
+      <c r="O34" t="str">
+        <f t="shared" si="26"/>
+        <v>-0,126216195408805, -0,658935195436524, -1,52071291472847, -2,58854511645354, -3,81350073815831, -5,17012847913034, -6,64372602703941, -8,2256630497373, -9,91134950997357, -11,6993410151046, -13,591081957774, -15,5911623752322, -17,7082125996275, -19,95693494329</v>
+      </c>
+      <c r="P34" t="str">
+        <f t="shared" si="26"/>
+        <v>-0,126216195408805, -0,658935195436524, -1,52071291472847, -2,58854511645354, -3,81350073815831, -5,17012847913034, -6,64372602703941, -8,2256630497373, -9,91134950997357, -11,6993410151046, -13,591081957774, -15,5911623752322, -17,7082125996275, -19,95693494329, -22,3627807069322</v>
+      </c>
+      <c r="Q34" t="str">
+        <f t="shared" si="26"/>
+        <v>-0,126216195408805, -0,658935195436524, -1,52071291472847, -2,58854511645354, -3,81350073815831, -5,17012847913034, -6,64372602703941, -8,2256630497373, -9,91134950997357, -11,6993410151046, -13,591081957774, -15,5911623752322, -17,7082125996275, -19,95693494329, -22,3627807069322, -24,9746809530075</v>
+      </c>
+      <c r="R34" t="str">
+        <f t="shared" si="26"/>
+        <v>-0,126216195408805, -0,658935195436524, -1,52071291472847, -2,58854511645354, -3,81350073815831, -5,17012847913034, -6,64372602703941, -8,2256630497373, -9,91134950997357, -11,6993410151046, -13,591081957774, -15,5911623752322, -17,7082125996275, -19,95693494329, -22,3627807069322, -24,9746809530075, -27,9156399183471</v>
+      </c>
+    </row>
+    <row r="35" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <f t="shared" si="25"/>
+        <v>-0.27642579730327427</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" si="26"/>
+        <v>-0,276425797303274, -0,463964595289396</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="26"/>
+        <v>-0,276425797303274, -0,463964595289396, -0,980562112539742</v>
+      </c>
+      <c r="E35" t="str">
+        <f t="shared" si="26"/>
+        <v>-0,276425797303274, -0,463964595289396, -0,980562112539742, -1,70321411222321</v>
+      </c>
+      <c r="F35" t="str">
+        <f t="shared" si="26"/>
+        <v>-0,276425797303274, -0,463964595289396, -0,980562112539742, -1,70321411222321, -2,58298953188638</v>
+      </c>
+      <c r="G35" t="str">
+        <f t="shared" si="26"/>
+        <v>-0,276425797303274, -0,463964595289396, -0,980562112539742, -1,70321411222321, -2,58298953188638, -3,59443707081682</v>
+      </c>
+      <c r="H35" t="str">
+        <f t="shared" si="26"/>
+        <v>-0,276425797303274, -0,463964595289396, -0,980562112539742, -1,70321411222321, -2,58298953188638, -3,59443707081682, -4,72285441668429</v>
+      </c>
+      <c r="I35" t="str">
+        <f t="shared" si="26"/>
+        <v>-0,276425797303274, -0,463964595289396, -0,980562112539742, -1,70321411222321, -2,58298953188638, -3,59443707081682, -4,72285441668429, -5,95961123734059</v>
+      </c>
+      <c r="J35" t="str">
+        <f t="shared" si="26"/>
+        <v>-0,276425797303274, -0,463964595289396, -0,980562112539742, -1,70321411222321, -2,58298953188638, -3,59443707081682, -4,72285441668429, -5,95961123734059, -7,30011749553526</v>
+      </c>
+      <c r="K35" t="str">
+        <f t="shared" si="26"/>
+        <v>-0,276425797303274, -0,463964595289396, -0,980562112539742, -1,70321411222321, -2,58298953188638, -3,59443707081682, -4,72285441668429, -5,95961123734059, -7,30011749553526, -8,74292879862468</v>
+      </c>
+      <c r="L35" t="str">
+        <f t="shared" si="26"/>
+        <v>-0,276425797303274, -0,463964595289396, -0,980562112539742, -1,70321411222321, -2,58298953188638, -3,59443707081682, -4,72285441668429, -5,95961123734059, -7,30011749553526, -8,74292879862468, -10,2894895392525</v>
+      </c>
+      <c r="M35" t="str">
+        <f t="shared" si="26"/>
+        <v>-0,276425797303274, -0,463964595289396, -0,980562112539742, -1,70321411222321, -2,58298953188638, -3,59443707081682, -4,72285441668429, -5,95961123734059, -7,30011749553526, -8,74292879862468, -10,2894895392525, -11,9443897546691</v>
+      </c>
+      <c r="N35" t="str">
+        <f t="shared" si="26"/>
+        <v>-0,276425797303274, -0,463964595289396, -0,980562112539742, -1,70321411222321, -2,58298953188638, -3,59443707081682, -4,72285441668429, -5,95961123734059, -7,30011749553526, -8,74292879862468, -10,2894895392525, -11,9443897546691, -13,7162597770228</v>
+      </c>
+      <c r="O35" t="str">
+        <f t="shared" si="26"/>
+        <v>-0,276425797303274, -0,463964595289396, -0,980562112539742, -1,70321411222321, -2,58298953188638, -3,59443707081682, -4,72285441668429, -5,95961123734059, -7,30011749553526, -8,74292879862468, -10,2894895392525, -11,9443897546691, -13,7162597770228, -15,6198019186437</v>
+      </c>
+      <c r="P35" t="str">
+        <f t="shared" si="26"/>
+        <v>-0,276425797303274, -0,463964595289396, -0,980562112539742, -1,70321411222321, -2,58298953188638, -3,59443707081682, -4,72285441668429, -5,95961123734059, -7,30011749553526, -8,74292879862468, -10,2894895392525, -11,9443897546691, -13,7162597770228, -15,6198019186437, -17,6804674802443</v>
+      </c>
+      <c r="Q35" t="str">
+        <f t="shared" si="26"/>
+        <v>-0,276425797303274, -0,463964595289396, -0,980562112539742, -1,70321411222321, -2,58298953188638, -3,59443707081682, -4,72285441668429, -5,95961123734059, -7,30011749553526, -8,74292879862468, -10,2894895392525, -11,9443897546691, -13,7162597770228, -15,6198019186437, -17,6804674802443, -19,947187524278</v>
+      </c>
+      <c r="R35" t="str">
+        <f t="shared" si="26"/>
+        <v>-0,276425797303274, -0,463964595289396, -0,980562112539742, -1,70321411222321, -2,58298953188638, -3,59443707081682, -4,72285441668429, -5,95961123734059, -7,30011749553526, -8,74292879862468, -10,2894895392525, -11,9443897546691, -13,7162597770228, -15,6198019186437, -17,6804674802443, -19,947187524278, -22,542966287576</v>
+      </c>
+    </row>
+    <row r="36" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <f t="shared" si="25"/>
+        <v>-0.57939476247111577</v>
+      </c>
+      <c r="C36" t="str">
+        <f t="shared" si="26"/>
+        <v>-0,579394762471116, -0,435972620168803</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="26"/>
+        <v>-0,579394762471116, -0,435972620168803, -0,621609197130714</v>
+      </c>
+      <c r="E36" t="str">
+        <f t="shared" si="26"/>
+        <v>-0,579394762471116, -0,435972620168803, -0,621609197130714, -1,01330025652575</v>
+      </c>
+      <c r="F36" t="str">
+        <f t="shared" si="26"/>
+        <v>-0,579394762471116, -0,435972620168803, -0,621609197130714, -1,01330025652575, -1,56211473590049</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" si="26"/>
+        <v>-0,579394762471116, -0,435972620168803, -0,621609197130714, -1,01330025652575, -1,56211473590049, -2,24260133454249</v>
+      </c>
+      <c r="H36" t="str">
+        <f t="shared" si="26"/>
+        <v>-0,579394762471116, -0,435972620168803, -0,621609197130714, -1,01330025652575, -1,56211473590049, -2,24260133454249, -3,04005774012152</v>
+      </c>
+      <c r="I36" t="str">
+        <f t="shared" si="26"/>
+        <v>-0,579394762471116, -0,435972620168803, -0,621609197130714, -1,01330025652575, -1,56211473590049, -2,24260133454249, -3,04005774012152, -3,94585362048939</v>
+      </c>
+      <c r="J36" t="str">
+        <f t="shared" si="26"/>
+        <v>-0,579394762471116, -0,435972620168803, -0,621609197130714, -1,01330025652575, -1,56211473590049, -2,24260133454249, -3,04005774012152, -3,94585362048939, -4,95539893839562</v>
+      </c>
+      <c r="K36" t="str">
+        <f t="shared" si="26"/>
+        <v>-0,579394762471116, -0,435972620168803, -0,621609197130714, -1,01330025652575, -1,56211473590049, -2,24260133454249, -3,04005774012152, -3,94585362048939, -4,95539893839562, -6,06724930119662</v>
+      </c>
+      <c r="L36" t="str">
+        <f t="shared" si="26"/>
+        <v>-0,579394762471116, -0,435972620168803, -0,621609197130714, -1,01330025652575, -1,56211473590049, -2,24260133454249, -3,04005774012152, -3,94585362048939, -4,95539893839562, -6,06724930119662, -7,28284910153597</v>
+      </c>
+      <c r="M36" t="str">
+        <f t="shared" si="26"/>
+        <v>-0,579394762471116, -0,435972620168803, -0,621609197130714, -1,01330025652575, -1,56211473590049, -2,24260133454249, -3,04005774012152, -3,94585362048939, -4,95539893839562, -6,06724930119662, -7,28284910153597, -8,60678837666416</v>
+      </c>
+      <c r="N36" t="str">
+        <f t="shared" si="26"/>
+        <v>-0,579394762471116, -0,435972620168803, -0,621609197130714, -1,01330025652575, -1,56211473590049, -2,24260133454249, -3,04005774012152, -3,94585362048939, -4,95539893839562, -6,06724930119662, -7,28284910153597, -8,60678837666416, -10,0476974587294</v>
+      </c>
+      <c r="O36" t="str">
+        <f t="shared" si="26"/>
+        <v>-0,579394762471116, -0,435972620168803, -0,621609197130714, -1,01330025652575, -1,56211473590049, -2,24260133454249, -3,04005774012152, -3,94585362048939, -4,95539893839562, -6,06724930119662, -7,28284910153597, -8,60678837666416, -10,0476974587294, -11,6202786600619</v>
+      </c>
+      <c r="P36" t="str">
+        <f t="shared" si="26"/>
+        <v>-0,579394762471116, -0,435972620168803, -0,621609197130714, -1,01330025652575, -1,56211473590049, -2,24260133454249, -3,04005774012152, -3,94585362048939, -4,95539893839562, -6,06724930119662, -7,28284910153597, -8,60678837666416, -10,0476974587294, -11,6202786600619, -13,3499832813741</v>
+      </c>
+      <c r="Q36" t="str">
+        <f t="shared" si="26"/>
+        <v>-0,579394762471116, -0,435972620168803, -0,621609197130714, -1,01330025652575, -1,56211473590049, -2,24260133454249, -3,04005774012152, -3,94585362048939, -4,95539893839562, -6,06724930119662, -7,28284910153597, -8,60678837666416, -10,0476974587294, -11,6202786600619, -13,3499832813741, -15,2857423851194</v>
+      </c>
+      <c r="R36" t="str">
+        <f t="shared" si="26"/>
+        <v>-0,579394762471116, -0,435972620168803, -0,621609197130714, -1,01330025652575, -1,56211473590049, -2,24260133454249, -3,04005774012152, -3,94585362048939, -4,95539893839562, -6,06724930119662, -7,28284910153597, -8,60678837666416, -10,0476974587294, -11,6202786600619, -13,3499832813741, -15,2857423851194, -17,5505602081289</v>
+      </c>
+    </row>
+    <row r="37" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <f t="shared" si="25"/>
+        <v>-4.8164799306236992</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" si="26"/>
         <v>-4,8164799306237, -3,61235994796777</v>
       </c>
-      <c r="D28" t="str">
-        <f t="shared" si="19"/>
+      <c r="D37" t="str">
+        <f t="shared" si="26"/>
         <v>-4,8164799306237, -3,61235994796777, -2,73729868457607</v>
       </c>
-      <c r="E28" t="str">
-        <f t="shared" si="19"/>
+      <c r="E37" t="str">
+        <f t="shared" si="26"/>
         <v>-4,8164799306237, -3,61235994796777, -2,73729868457607, -2,0682919036175</v>
       </c>
-      <c r="F28" t="str">
-        <f t="shared" si="19"/>
+      <c r="F37" t="str">
+        <f t="shared" si="26"/>
         <v>-4,8164799306237, -3,61235994796777, -2,73729868457607, -2,0682919036175, -1,55640854263862</v>
       </c>
-      <c r="G28" t="str">
-        <f t="shared" si="19"/>
+      <c r="G37" t="str">
+        <f t="shared" si="26"/>
         <v>-4,8164799306237, -3,61235994796777, -2,73729868457607, -2,0682919036175, -1,55640854263862, -1,17619730092702</v>
       </c>
-      <c r="H28" t="str">
-        <f t="shared" si="19"/>
+      <c r="H37" t="str">
+        <f t="shared" si="26"/>
         <v>-4,8164799306237, -3,61235994796777, -2,73729868457607, -2,0682919036175, -1,55640854263862, -1,17619730092702, -0,912955866152437</v>
       </c>
-      <c r="I28" t="str">
-        <f t="shared" si="19"/>
+      <c r="I37" t="str">
+        <f t="shared" si="26"/>
         <v>-4,8164799306237, -3,61235994796777, -2,73729868457607, -2,0682919036175, -1,55640854263862, -1,17619730092702, -0,912955866152437, -0,758053906166694</v>
       </c>
-      <c r="J28" t="str">
-        <f t="shared" si="19"/>
+      <c r="J37" t="str">
+        <f t="shared" si="26"/>
         <v>-4,8164799306237, -3,61235994796777, -2,73729868457607, -2,0682919036175, -1,55640854263862, -1,17619730092702, -0,912955866152437, -0,758053906166694, -0,706901383719312</v>
       </c>
-      <c r="K28" t="str">
-        <f t="shared" si="19"/>
+      <c r="K37" t="str">
+        <f t="shared" si="26"/>
         <v>-4,8164799306237, -3,61235994796777, -2,73729868457607, -2,0682919036175, -1,55640854263862, -1,17619730092702, -0,912955866152437, -0,758053906166694, -0,706901383719312, -0,758053906166694</v>
       </c>
-      <c r="L28" t="str">
-        <f t="shared" si="19"/>
+      <c r="L37" t="str">
+        <f t="shared" si="26"/>
         <v>-4,8164799306237, -3,61235994796777, -2,73729868457607, -2,0682919036175, -1,55640854263862, -1,17619730092702, -0,912955866152437, -0,758053906166694, -0,706901383719312, -0,758053906166694, -0,912955866152437</v>
       </c>
-      <c r="M28" t="str">
-        <f t="shared" si="19"/>
+      <c r="M37" t="str">
+        <f t="shared" si="26"/>
         <v>-4,8164799306237, -3,61235994796777, -2,73729868457607, -2,0682919036175, -1,55640854263862, -1,17619730092702, -0,912955866152437, -0,758053906166694, -0,706901383719312, -0,758053906166694, -0,912955866152437, -1,17619730092702</v>
       </c>
-      <c r="N28" t="str">
-        <f t="shared" si="19"/>
+      <c r="N37" t="str">
+        <f t="shared" si="26"/>
         <v>-4,8164799306237, -3,61235994796777, -2,73729868457607, -2,0682919036175, -1,55640854263862, -1,17619730092702, -0,912955866152437, -0,758053906166694, -0,706901383719312, -0,758053906166694, -0,912955866152437, -1,17619730092702, -1,55640854263862</v>
       </c>
-      <c r="O28" t="str">
-        <f t="shared" si="19"/>
+      <c r="O37" t="str">
+        <f t="shared" si="26"/>
         <v>-4,8164799306237, -3,61235994796777, -2,73729868457607, -2,0682919036175, -1,55640854263862, -1,17619730092702, -0,912955866152437, -0,758053906166694, -0,706901383719312, -0,758053906166694, -0,912955866152437, -1,17619730092702, -1,55640854263862, -2,0682919036175</v>
       </c>
-      <c r="P28" t="str">
-        <f t="shared" si="19"/>
+      <c r="P37" t="str">
+        <f t="shared" si="26"/>
         <v>-4,8164799306237, -3,61235994796777, -2,73729868457607, -2,0682919036175, -1,55640854263862, -1,17619730092702, -0,912955866152437, -0,758053906166694, -0,706901383719312, -0,758053906166694, -0,912955866152437, -1,17619730092702, -1,55640854263862, -2,0682919036175, -2,73729868457607</v>
       </c>
-      <c r="Q28" t="str">
-        <f t="shared" si="19"/>
+      <c r="Q37" t="str">
+        <f t="shared" si="26"/>
         <v>-4,8164799306237, -3,61235994796777, -2,73729868457607, -2,0682919036175, -1,55640854263862, -1,17619730092702, -0,912955866152437, -0,758053906166694, -0,706901383719312, -0,758053906166694, -0,912955866152437, -1,17619730092702, -1,55640854263862, -2,0682919036175, -2,73729868457607, -3,61235994796777</v>
       </c>
-      <c r="R28" t="str">
-        <f t="shared" si="19"/>
+      <c r="R37" t="str">
+        <f t="shared" si="26"/>
         <v>-4,8164799306237, -3,61235994796777, -2,73729868457607, -2,0682919036175, -1,55640854263862, -1,17619730092702, -0,912955866152437, -0,758053906166694, -0,706901383719312, -0,758053906166694, -0,912955866152437, -1,17619730092702, -1,55640854263862, -2,0682919036175, -2,73729868457607, -3,61235994796777, -4,8164799306237</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>